<commit_message>
Dynamic licences; full run of spreadsheet prep
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30500" windowHeight="19140" activeTab="1"/>
+    <workbookView xWindow="20480" yWindow="0" windowWidth="20480" windowHeight="22580"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3909" uniqueCount="3739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="3747">
   <si>
     <t>1r</t>
   </si>
@@ -11276,15 +11276,46 @@
   </si>
   <si>
     <t>1909</t>
+  </si>
+  <si>
+    <t>ourID</t>
+  </si>
+  <si>
+    <t>From January 1, 1903 to March 26, 1909</t>
+  </si>
+  <si>
+    <t>205 x 150 mm</t>
+  </si>
+  <si>
+    <t>215 x 162 mm</t>
+  </si>
+  <si>
+    <t>http://www.example.com/facsimile</t>
+  </si>
+  <si>
+    <t>Facsimile</t>
+  </si>
+  <si>
+    <t>Smith, John (1843-1909)</t>
+  </si>
+  <si>
+    <t>httt://example.com/JohnSmith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -11408,84 +11439,85 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -11838,11 +11870,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12280,7 +12312,9 @@
       <c r="B20" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4">
+        <v>1234567</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -12308,7 +12342,9 @@
       <c r="B21" s="5" t="s">
         <v>3657</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>3739</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -12347,7 +12383,9 @@
       <c r="B23" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4">
+        <v>2</v>
+      </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -12481,6 +12519,9 @@
       <c r="B30" s="5" t="s">
         <v>2664</v>
       </c>
+      <c r="C30" s="23" t="s">
+        <v>3740</v>
+      </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -12557,6 +12598,9 @@
       <c r="B38" s="5" t="s">
         <v>2664</v>
       </c>
+      <c r="C38" s="23" t="s">
+        <v>3741</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="4" t="s">
@@ -12565,6 +12609,9 @@
       <c r="B39" s="5" t="s">
         <v>2664</v>
       </c>
+      <c r="C39" s="23" t="s">
+        <v>3742</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
@@ -12573,7 +12620,9 @@
       <c r="B41" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="23" t="s">
+        <v>3744</v>
+      </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
@@ -12582,6 +12631,9 @@
       <c r="B42" s="5" t="s">
         <v>2664</v>
       </c>
+      <c r="C42" s="18" t="s">
+        <v>3743</v>
+      </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
@@ -12590,7 +12642,9 @@
       <c r="B44" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="23" t="s">
+        <v>3745</v>
+      </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
@@ -12602,6 +12656,9 @@
       </c>
       <c r="B45" s="5" t="s">
         <v>2664</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>3746</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -12908,6 +12965,7 @@
     <hyperlink ref="C9" r:id="rId1"/>
     <hyperlink ref="C15" r:id="rId2"/>
     <hyperlink ref="C54" r:id="rId3"/>
+    <hyperlink ref="C42" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -12939,7 +12997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>

</xml_diff>

<commit_message>
TEI fixes: multiple collections, vol nos. in title, call number; keywords: remove periods.
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="3747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3918" uniqueCount="3748">
   <si>
     <t>1r</t>
   </si>
@@ -11300,15 +11300,25 @@
   </si>
   <si>
     <t>httt://example.com/JohnSmith</t>
+  </si>
+  <si>
+    <t>Diaries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -11437,89 +11447,92 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -11547,6 +11560,8 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -11871,10 +11886,10 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44:C45"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12184,7 +12199,7 @@
       <c r="C15" s="18" t="s">
         <v>3677</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -12273,6 +12288,9 @@
       </c>
       <c r="C18" s="17" t="s">
         <v>3713</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>3747</v>
       </c>
     </row>
     <row r="19" spans="1:22">

</xml_diff>

<commit_message>
Add multiple languages to test fixture
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3918" uniqueCount="3748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3920" uniqueCount="3748">
   <si>
     <t>1r</t>
   </si>
@@ -11886,10 +11886,10 @@
   <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12591,6 +12591,12 @@
       </c>
       <c r="C34" s="17" t="s">
         <v>2935</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>3411</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>2723</v>
       </c>
     </row>
     <row r="36" spans="1:7">

</xml_diff>

<commit_message>
Add calc'd full shelf mark; fix bug in op-prep.py
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
@@ -11901,7 +11901,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD23"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12370,7 +12370,9 @@
       <c r="B21" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4">
+        <v>2</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -12398,7 +12400,9 @@
       <c r="B22" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4">
+        <v>3</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>

</xml_diff>

<commit_message>
Handle and clean Unicode in spreadsheets
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3928" uniqueCount="3752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3932" uniqueCount="3754">
   <si>
     <t>1r</t>
   </si>
@@ -11315,13 +11315,19 @@
   </si>
   <si>
     <t>Archival Item</t>
+  </si>
+  <si>
+    <t>בראשית ברא אלהים</t>
+  </si>
+  <si>
+    <t>“Here’s some ‘smart’ quotes.”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11423,6 +11429,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Myriad Hebrew Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -11513,7 +11530,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -11543,6 +11560,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -11897,7 +11918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -13153,9 +13174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13241,7 +13262,7 @@
         <v>3685</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="15">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -13257,8 +13278,14 @@
       <c r="F5" s="15" t="s">
         <v>3686</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="G5" s="2" t="s">
+        <v>2618</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -13273,6 +13300,12 @@
       </c>
       <c r="F6" s="15" t="s">
         <v>3687</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>2618</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>3753</v>
       </c>
     </row>
     <row r="7" spans="1:12">

</xml_diff>

<commit_message>
Allow CC-BY-SA for diaries
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
+++ b/openn/tests/data/sheets/valid_template/openn_metadata.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3934" uniqueCount="3756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3935" uniqueCount="3757">
   <si>
     <t>1r</t>
   </si>
@@ -11335,6 +11335,9 @@
   </si>
   <si>
     <t>resource</t>
+  </si>
+  <si>
+    <t>CC-BY-SA</t>
   </si>
 </sst>
 </file>
@@ -11933,10 +11936,10 @@
   <dimension ref="A1:V66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13029,7 +13032,7 @@
         <v>2656</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>2674</v>
+        <v>3756</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
@@ -30993,7 +30996,7 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31043,6 +31046,9 @@
       <c r="B6" t="s">
         <v>2620</v>
       </c>
+      <c r="D6" t="s">
+        <v>3756</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">

</xml_diff>